<commit_message>
added back response curve functionality
</commit_message>
<xml_diff>
--- a/summaryFrame.xlsx
+++ b/summaryFrame.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Y1_1</t>
+          <t>2020_1</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -504,7 +504,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Y1_2</t>
+          <t>2020_2</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -532,7 +532,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Y1_3</t>
+          <t>2020_3</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -560,7 +560,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Y1_4</t>
+          <t>2020_4</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -588,7 +588,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Y1_5</t>
+          <t>2020_5</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -616,7 +616,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Y1_6</t>
+          <t>2020_6</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -646,7 +646,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Y1_7</t>
+          <t>2020_7</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -676,7 +676,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Y1_8</t>
+          <t>2020_8</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -706,7 +706,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Y1_9</t>
+          <t>2020_9</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -736,7 +736,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Y1_10</t>
+          <t>2020_10</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -756,10 +756,8 @@
       <c r="G11" t="n">
         <v>0.1003029380720502</v>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -768,7 +766,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Y1_11</t>
+          <t>2020_11</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -788,10 +786,8 @@
       <c r="G12" t="n">
         <v>0.06655132593534674</v>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -800,7 +796,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Y1_12</t>
+          <t>2020_12</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -820,10 +816,8 @@
       <c r="G13" t="n">
         <v>0.03250137842916226</v>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -832,7 +826,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Y1_13</t>
+          <t>2020_13</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -860,7 +854,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Y1_14</t>
+          <t>2020_14</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -890,7 +884,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Y1_15</t>
+          <t>2020_15</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -920,7 +914,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Y1_16</t>
+          <t>2020_16</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -950,7 +944,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Y1_17</t>
+          <t>2020_17</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -980,7 +974,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Y1_18</t>
+          <t>2020_18</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1000,10 +994,8 @@
       <c r="G19" t="n">
         <v>0.07773753564207328</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1012,7 +1004,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Y1_19</t>
+          <t>2020_19</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1032,10 +1024,8 @@
       <c r="G20" t="n">
         <v>0.0501242191949469</v>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1044,7 +1034,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Y1_20</t>
+          <t>2020_20</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1064,10 +1054,8 @@
       <c r="G21" t="n">
         <v>0.02431060411729764</v>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1076,7 +1064,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Y1_21</t>
+          <t>2020_21</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1104,7 +1092,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Y1_22</t>
+          <t>2020_22</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1134,7 +1122,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Y1_23</t>
+          <t>2020_23</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1164,7 +1152,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Y1_24</t>
+          <t>2020_24</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1194,7 +1182,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Y1_25</t>
+          <t>2020_25</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1224,7 +1212,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Y1_26</t>
+          <t>2020_26</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1254,7 +1242,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Y1_27</t>
+          <t>2020_27</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1284,7 +1272,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Y1_28</t>
+          <t>2020_28</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1304,10 +1292,8 @@
       <c r="G29" t="n">
         <v>0.144559753400299</v>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1316,7 +1302,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Y1_29</t>
+          <t>2020_29</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1336,10 +1322,8 @@
       <c r="G30" t="n">
         <v>0.0918009811071815</v>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1348,7 +1332,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Y1_30</t>
+          <t>2020_30</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1378,7 +1362,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Y1_31</t>
+          <t>2020_31</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1408,7 +1392,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Y1_32</t>
+          <t>2020_32</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1438,7 +1422,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Y1_33</t>
+          <t>2020_33</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1468,7 +1452,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Y1_34</t>
+          <t>2020_34</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1488,10 +1472,8 @@
       <c r="G35" t="n">
         <v>0.1004413636346295</v>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1500,7 +1482,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Y1_35</t>
+          <t>2020_35</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1520,10 +1502,8 @@
       <c r="G36" t="n">
         <v>0.0666466222227028</v>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1532,7 +1512,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Y1_36</t>
+          <t>2020_36</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1552,10 +1532,8 @@
       <c r="G37" t="n">
         <v>0.03254961802339342</v>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1564,7 +1542,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Y1_37</t>
+          <t>2020_37</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1592,7 +1570,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Y1_38</t>
+          <t>2020_38</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1622,7 +1600,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Y1_39</t>
+          <t>2020_39</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1652,7 +1630,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Y1_40</t>
+          <t>2020_40</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1682,7 +1660,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Y1_41</t>
+          <t>2020_41</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1712,7 +1690,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Y1_42</t>
+          <t>2020_42</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1732,10 +1710,8 @@
       <c r="G43" t="n">
         <v>0.08400787436820399</v>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1744,7 +1720,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Y1_43</t>
+          <t>2020_43</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1764,10 +1740,8 @@
       <c r="G44" t="n">
         <v>0.06416429281940138</v>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1776,7 +1750,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Y1_44</t>
+          <t>2020_44</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1796,10 +1770,8 @@
       <c r="G45" t="n">
         <v>0.03244096535198271</v>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1808,7 +1780,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Y1_45</t>
+          <t>2020_45</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1836,7 +1808,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Y1_46</t>
+          <t>2020_46</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1866,7 +1838,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Y1_47</t>
+          <t>2020_47</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1896,7 +1868,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Y1_48</t>
+          <t>2020_48</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1926,7 +1898,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Y2_1</t>
+          <t>2021_1</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1956,7 +1928,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Y2_2</t>
+          <t>2021_2</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1986,7 +1958,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Y2_3</t>
+          <t>2021_3</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -2016,7 +1988,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Y2_4</t>
+          <t>2021_4</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -2046,7 +2018,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Y2_5</t>
+          <t>2021_5</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -2076,7 +2048,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Y2_6</t>
+          <t>2021_6</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -2106,7 +2078,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Y2_7</t>
+          <t>2021_7</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -2136,7 +2108,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Y2_8</t>
+          <t>2021_8</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2166,7 +2138,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Y2_9</t>
+          <t>2021_9</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2196,7 +2168,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Y2_10</t>
+          <t>2021_10</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -2216,10 +2188,8 @@
       <c r="G59" t="n">
         <v>0.07770528201974378</v>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2228,7 +2198,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Y2_11</t>
+          <t>2021_11</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -2248,10 +2218,8 @@
       <c r="G60" t="n">
         <v>0.05010369519394205</v>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2260,7 +2228,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Y2_12</t>
+          <t>2021_12</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -2280,10 +2248,8 @@
       <c r="G61" t="n">
         <v>0.02430038301333078</v>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2292,7 +2258,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Y2_13</t>
+          <t>2021_13</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -2320,7 +2286,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Y2_14</t>
+          <t>2021_14</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -2350,7 +2316,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Y2_15</t>
+          <t>2021_15</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -2380,7 +2346,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Y2_16</t>
+          <t>2021_16</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -2410,7 +2376,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Y2_17</t>
+          <t>2021_17</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -2440,7 +2406,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Y2_18</t>
+          <t>2021_18</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -2460,10 +2426,8 @@
       <c r="G67" t="n">
         <v>0.1003670242559912</v>
       </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2472,7 +2436,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Y2_19</t>
+          <t>2021_19</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -2492,10 +2456,8 @@
       <c r="G68" t="n">
         <v>0.06659544354975346</v>
       </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H68" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2504,7 +2466,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Y2_20</t>
+          <t>2021_20</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -2524,10 +2486,8 @@
       <c r="G69" t="n">
         <v>0.0325237104231475</v>
       </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2536,7 +2496,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Y2_21</t>
+          <t>2021_21</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -2564,7 +2524,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Y2_22</t>
+          <t>2021_22</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -2594,7 +2554,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Y2_23</t>
+          <t>2021_23</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -2624,7 +2584,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Y2_24</t>
+          <t>2021_24</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -2654,7 +2614,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Y2_25</t>
+          <t>2021_25</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -2684,7 +2644,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Y2_26</t>
+          <t>2021_26</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -2704,10 +2664,8 @@
       <c r="G75" t="n">
         <v>0.1003877150638314</v>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2716,7 +2674,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Y2_27</t>
+          <t>2021_27</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -2736,10 +2694,8 @@
       <c r="G76" t="n">
         <v>0.06660968777480153</v>
       </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2748,7 +2704,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Y2_28</t>
+          <t>2021_28</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -2778,7 +2734,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Y2_29</t>
+          <t>2021_29</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -2808,7 +2764,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Y2_30</t>
+          <t>2021_30</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -2838,7 +2794,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Y2_31</t>
+          <t>2021_31</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -2868,7 +2824,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Y2_32</t>
+          <t>2021_32</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -2898,7 +2854,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Y2_33</t>
+          <t>2021_33</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -2928,7 +2884,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Y2_34</t>
+          <t>2021_34</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -2948,10 +2904,8 @@
       <c r="G83" t="n">
         <v>0.1051550937077204</v>
       </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2960,7 +2914,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Y2_35</t>
+          <t>2021_35</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -2980,10 +2934,8 @@
       <c r="G84" t="n">
         <v>0.0641752949118992</v>
       </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H84" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2992,7 +2944,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Y2_36</t>
+          <t>2021_36</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -3012,10 +2964,8 @@
       <c r="G85" t="n">
         <v>0.03244705173577779</v>
       </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H85" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -3024,7 +2974,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Y2_37</t>
+          <t>2021_37</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -3052,7 +3002,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Y2_38</t>
+          <t>2021_38</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -3082,7 +3032,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Y2_39</t>
+          <t>2021_39</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -3112,7 +3062,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Y2_40</t>
+          <t>2021_40</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -3142,7 +3092,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Y2_41</t>
+          <t>2021_41</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -3172,7 +3122,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Y2_42</t>
+          <t>2021_42</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -3192,10 +3142,8 @@
       <c r="G91" t="n">
         <v>0.1004237597362826</v>
       </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H91" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -3204,7 +3152,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Y2_43</t>
+          <t>2021_43</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -3224,10 +3172,8 @@
       <c r="G92" t="n">
         <v>0.06663450262618084</v>
       </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H92" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -3236,7 +3182,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Y2_44</t>
+          <t>2021_44</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -3256,10 +3202,8 @@
       <c r="G93" t="n">
         <v>0.03254348272589212</v>
       </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H93" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -3268,7 +3212,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Y2_45</t>
+          <t>2021_45</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -3296,7 +3240,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Y2_46</t>
+          <t>2021_46</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -3326,7 +3270,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Y2_47</t>
+          <t>2021_47</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -3356,7 +3300,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Y2_48</t>
+          <t>2021_48</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -3386,7 +3330,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Y3_1</t>
+          <t>2022_1</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -3416,7 +3360,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Y3_2</t>
+          <t>2022_2</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -3436,10 +3380,8 @@
       <c r="G99" t="n">
         <v>0.0777424212416223</v>
       </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H99" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3448,7 +3390,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Y3_3</t>
+          <t>2022_3</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -3468,10 +3410,8 @@
       <c r="G100" t="n">
         <v>0.05012732803712636</v>
       </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H100" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -3480,7 +3420,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Y3_4</t>
+          <t>2022_4</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -3500,10 +3440,8 @@
       <c r="G101" t="n">
         <v>0.02431215236322074</v>
       </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H101" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -3512,7 +3450,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Y3_5</t>
+          <t>2022_5</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -3540,7 +3478,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Y3_6</t>
+          <t>2022_6</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -3570,7 +3508,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Y3_7</t>
+          <t>2022_7</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -3600,7 +3538,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Y3_8</t>
+          <t>2022_8</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -3630,7 +3568,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Y3_9</t>
+          <t>2022_9</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -3660,7 +3598,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Y3_10</t>
+          <t>2022_10</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -3680,10 +3618,8 @@
       <c r="G107" t="n">
         <v>0.1733384996963195</v>
       </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H107" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -3692,7 +3628,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Y3_11</t>
+          <t>2022_11</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -3712,10 +3648,8 @@
       <c r="G108" t="n">
         <v>0.1296786812189736</v>
       </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H108" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -3724,7 +3658,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Y3_12</t>
+          <t>2022_12</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -3744,10 +3678,8 @@
       <c r="G109" t="n">
         <v>0.07223125345513458</v>
       </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H109" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -3756,7 +3688,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Y3_13</t>
+          <t>2022_13</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -3784,7 +3716,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Y3_14</t>
+          <t>2022_14</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -3814,7 +3746,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Y3_15</t>
+          <t>2022_15</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -3844,7 +3776,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Y3_16</t>
+          <t>2022_16</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -3874,7 +3806,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Y3_17</t>
+          <t>2022_17</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -3904,7 +3836,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Y3_18</t>
+          <t>2022_18</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -3924,10 +3856,8 @@
       <c r="G115" t="n">
         <v>0.1003670242559912</v>
       </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H115" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -3936,7 +3866,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Y3_19</t>
+          <t>2022_19</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -3956,10 +3886,8 @@
       <c r="G116" t="n">
         <v>0.06659544354975346</v>
       </c>
-      <c r="H116" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H116" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -3968,7 +3896,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Y3_20</t>
+          <t>2022_20</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -3988,10 +3916,8 @@
       <c r="G117" t="n">
         <v>0.0325237104231475</v>
       </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H117" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -4000,7 +3926,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Y3_21</t>
+          <t>2022_21</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -4028,7 +3954,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Y3_22</t>
+          <t>2022_22</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -4058,7 +3984,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Y3_23</t>
+          <t>2022_23</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -4088,7 +4014,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Y3_24</t>
+          <t>2022_24</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -4118,7 +4044,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Y3_25</t>
+          <t>2022_25</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -4148,7 +4074,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Y3_26</t>
+          <t>2022_26</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -4168,10 +4094,8 @@
       <c r="G123" t="n">
         <v>0.0839853763852647</v>
       </c>
-      <c r="H123" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H123" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -4180,7 +4104,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Y3_27</t>
+          <t>2022_27</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -4200,10 +4124,8 @@
       <c r="G124" t="n">
         <v>0.06414176534060709</v>
       </c>
-      <c r="H124" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H124" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -4212,7 +4134,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Y3_28</t>
+          <t>2022_28</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -4232,10 +4154,8 @@
       <c r="G125" t="n">
         <v>0.03242850371012066</v>
       </c>
-      <c r="H125" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H125" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -4244,7 +4164,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Y3_29</t>
+          <t>2022_29</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -4272,7 +4192,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Y3_30</t>
+          <t>2022_30</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -4302,7 +4222,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Y3_31</t>
+          <t>2022_31</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -4332,7 +4252,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Y3_32</t>
+          <t>2022_32</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -4362,7 +4282,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Y3_33</t>
+          <t>2022_33</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -4392,7 +4312,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Y3_34</t>
+          <t>2022_34</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -4422,7 +4342,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Y3_35</t>
+          <t>2022_35</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -4452,7 +4372,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Y3_36</t>
+          <t>2022_36</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -4472,10 +4392,8 @@
       <c r="G133" t="n">
         <v>0.1446332128874222</v>
       </c>
-      <c r="H133" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H133" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -4484,7 +4402,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Y3_37</t>
+          <t>2022_37</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -4504,10 +4422,8 @@
       <c r="G134" t="n">
         <v>0.09162681059707677</v>
       </c>
-      <c r="H134" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H134" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -4516,7 +4432,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Y3_38</t>
+          <t>2022_38</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -4546,7 +4462,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Y3_39</t>
+          <t>2022_39</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -4576,7 +4492,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Y3_40</t>
+          <t>2022_40</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -4606,7 +4522,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Y3_41</t>
+          <t>2022_41</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -4636,7 +4552,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Y3_42</t>
+          <t>2022_42</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -4656,10 +4572,8 @@
       <c r="G139" t="n">
         <v>0.07776607772423155</v>
       </c>
-      <c r="H139" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H139" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -4668,7 +4582,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Y3_43</t>
+          <t>2022_43</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -4688,10 +4602,8 @@
       <c r="G140" t="n">
         <v>0.05014238123908044</v>
       </c>
-      <c r="H140" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H140" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -4700,7 +4612,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Y3_44</t>
+          <t>2022_44</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -4720,10 +4632,8 @@
       <c r="G141" t="n">
         <v>0.02431964913650792</v>
       </c>
-      <c r="H141" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H141" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -4732,7 +4642,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Y3_45</t>
+          <t>2022_45</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -4760,7 +4670,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Y3_46</t>
+          <t>2022_46</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -4788,7 +4698,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Y3_47</t>
+          <t>2022_47</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -4816,7 +4726,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Y3_48</t>
+          <t>2022_48</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -4844,7 +4754,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Y1_1</t>
+          <t>2020_1</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -4872,7 +4782,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Y1_2</t>
+          <t>2020_2</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -4900,7 +4810,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Y1_3</t>
+          <t>2020_3</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -4928,7 +4838,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Y1_4</t>
+          <t>2020_4</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -4956,7 +4866,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Y1_5</t>
+          <t>2020_5</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -4984,7 +4894,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Y1_6</t>
+          <t>2020_6</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -5012,7 +4922,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Y1_7</t>
+          <t>2020_7</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -5040,7 +4950,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Y1_8</t>
+          <t>2020_8</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -5068,7 +4978,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Y1_9</t>
+          <t>2020_9</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -5096,7 +5006,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Y1_10</t>
+          <t>2020_10</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -5124,7 +5034,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Y1_11</t>
+          <t>2020_11</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -5152,7 +5062,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Y1_12</t>
+          <t>2020_12</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -5180,7 +5090,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Y1_13</t>
+          <t>2020_13</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -5208,7 +5118,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Y1_14</t>
+          <t>2020_14</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -5236,7 +5146,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Y1_15</t>
+          <t>2020_15</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -5264,7 +5174,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Y1_16</t>
+          <t>2020_16</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -5292,7 +5202,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Y1_17</t>
+          <t>2020_17</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -5320,7 +5230,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Y1_18</t>
+          <t>2020_18</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -5350,7 +5260,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Y1_19</t>
+          <t>2020_19</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -5380,7 +5290,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Y1_20</t>
+          <t>2020_20</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -5410,7 +5320,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Y1_21</t>
+          <t>2020_21</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -5440,7 +5350,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Y1_22</t>
+          <t>2020_22</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -5460,10 +5370,8 @@
       <c r="G167" t="n">
         <v>0.2509110206568765</v>
       </c>
-      <c r="H167" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H167" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -5472,7 +5380,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Y1_23</t>
+          <t>2020_23</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -5492,10 +5400,8 @@
       <c r="G168" t="n">
         <v>0.05482389318297983</v>
       </c>
-      <c r="H168" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H168" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -5504,7 +5410,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Y1_24</t>
+          <t>2020_24</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -5524,10 +5430,8 @@
       <c r="G169" t="n">
         <v>0.004384643015532226</v>
       </c>
-      <c r="H169" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H169" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -5536,7 +5440,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Y1_25</t>
+          <t>2020_25</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -5564,7 +5468,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Y1_26</t>
+          <t>2020_26</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -5592,7 +5496,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Y1_27</t>
+          <t>2020_27</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -5620,7 +5524,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Y1_28</t>
+          <t>2020_28</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -5648,7 +5552,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Y1_29</t>
+          <t>2020_29</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -5676,7 +5580,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Y1_30</t>
+          <t>2020_30</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -5704,7 +5608,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Y1_31</t>
+          <t>2020_31</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -5732,7 +5636,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Y1_32</t>
+          <t>2020_32</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -5760,7 +5664,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Y1_33</t>
+          <t>2020_33</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -5788,7 +5692,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Y1_34</t>
+          <t>2020_34</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -5816,7 +5720,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Y1_35</t>
+          <t>2020_35</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -5844,7 +5748,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Y1_36</t>
+          <t>2020_36</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -5872,7 +5776,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Y1_37</t>
+          <t>2020_37</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -5900,7 +5804,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Y1_38</t>
+          <t>2020_38</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -5930,7 +5834,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Y1_39</t>
+          <t>2020_39</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -5960,7 +5864,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Y1_40</t>
+          <t>2020_40</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -5990,7 +5894,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Y1_41</t>
+          <t>2020_41</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -6020,7 +5924,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Y1_42</t>
+          <t>2020_42</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -6040,10 +5944,8 @@
       <c r="G187" t="n">
         <v>0.2448455594779002</v>
       </c>
-      <c r="H187" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H187" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -6052,7 +5954,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Y1_43</t>
+          <t>2020_43</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -6072,10 +5974,8 @@
       <c r="G188" t="n">
         <v>0.05590364342310219</v>
       </c>
-      <c r="H188" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H188" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -6084,7 +5984,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Y1_44</t>
+          <t>2020_44</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -6104,10 +6004,8 @@
       <c r="G189" t="n">
         <v>0.004781788492240781</v>
       </c>
-      <c r="H189" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H189" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="190">
@@ -6116,7 +6014,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Y1_45</t>
+          <t>2020_45</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -6144,7 +6042,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Y1_46</t>
+          <t>2020_46</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -6172,7 +6070,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Y1_47</t>
+          <t>2020_47</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -6200,7 +6098,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Y1_48</t>
+          <t>2020_48</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -6228,7 +6126,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Y2_1</t>
+          <t>2021_1</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -6256,7 +6154,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Y2_2</t>
+          <t>2021_2</t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -6284,7 +6182,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Y2_3</t>
+          <t>2021_3</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -6312,7 +6210,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Y2_4</t>
+          <t>2021_4</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -6340,7 +6238,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Y2_5</t>
+          <t>2021_5</t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -6368,7 +6266,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Y2_6</t>
+          <t>2021_6</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -6396,7 +6294,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Y2_7</t>
+          <t>2021_7</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -6424,7 +6322,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Y2_8</t>
+          <t>2021_8</t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -6452,7 +6350,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Y2_9</t>
+          <t>2021_9</t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -6480,7 +6378,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Y2_10</t>
+          <t>2021_10</t>
         </is>
       </c>
       <c r="C203" t="n">
@@ -6510,7 +6408,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Y2_11</t>
+          <t>2021_11</t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -6540,7 +6438,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Y2_12</t>
+          <t>2021_12</t>
         </is>
       </c>
       <c r="C205" t="n">
@@ -6570,7 +6468,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Y2_13</t>
+          <t>2021_13</t>
         </is>
       </c>
       <c r="C206" t="n">
@@ -6600,7 +6498,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Y2_14</t>
+          <t>2021_14</t>
         </is>
       </c>
       <c r="C207" t="n">
@@ -6620,10 +6518,8 @@
       <c r="G207" t="n">
         <v>0.2508918428546285</v>
       </c>
-      <c r="H207" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H207" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="208">
@@ -6632,7 +6528,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Y2_15</t>
+          <t>2021_15</t>
         </is>
       </c>
       <c r="C208" t="n">
@@ -6652,10 +6548,8 @@
       <c r="G208" t="n">
         <v>0.05481877771718634</v>
       </c>
-      <c r="H208" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H208" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="209">
@@ -6664,7 +6558,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Y2_16</t>
+          <t>2021_16</t>
         </is>
       </c>
       <c r="C209" t="n">
@@ -6684,10 +6578,8 @@
       <c r="G209" t="n">
         <v>0.004509052058470252</v>
       </c>
-      <c r="H209" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H209" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -6696,7 +6588,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Y2_17</t>
+          <t>2021_17</t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -6724,7 +6616,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Y2_18</t>
+          <t>2021_18</t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -6752,7 +6644,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Y2_19</t>
+          <t>2021_19</t>
         </is>
       </c>
       <c r="C212" t="n">
@@ -6780,7 +6672,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Y2_20</t>
+          <t>2021_20</t>
         </is>
       </c>
       <c r="C213" t="n">
@@ -6808,7 +6700,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Y2_21</t>
+          <t>2021_21</t>
         </is>
       </c>
       <c r="C214" t="n">
@@ -6836,7 +6728,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Y2_22</t>
+          <t>2021_22</t>
         </is>
       </c>
       <c r="C215" t="n">
@@ -6864,7 +6756,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Y2_23</t>
+          <t>2021_23</t>
         </is>
       </c>
       <c r="C216" t="n">
@@ -6892,7 +6784,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Y2_24</t>
+          <t>2021_24</t>
         </is>
       </c>
       <c r="C217" t="n">
@@ -6920,7 +6812,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Y2_25</t>
+          <t>2021_25</t>
         </is>
       </c>
       <c r="C218" t="n">
@@ -6948,7 +6840,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Y2_26</t>
+          <t>2021_26</t>
         </is>
       </c>
       <c r="C219" t="n">
@@ -6976,7 +6868,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Y2_27</t>
+          <t>2021_27</t>
         </is>
       </c>
       <c r="C220" t="n">
@@ -7004,7 +6896,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Y2_28</t>
+          <t>2021_28</t>
         </is>
       </c>
       <c r="C221" t="n">
@@ -7032,7 +6924,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Y2_29</t>
+          <t>2021_29</t>
         </is>
       </c>
       <c r="C222" t="n">
@@ -7060,7 +6952,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Y2_30</t>
+          <t>2021_30</t>
         </is>
       </c>
       <c r="C223" t="n">
@@ -7090,7 +6982,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Y2_31</t>
+          <t>2021_31</t>
         </is>
       </c>
       <c r="C224" t="n">
@@ -7120,7 +7012,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Y2_32</t>
+          <t>2021_32</t>
         </is>
       </c>
       <c r="C225" t="n">
@@ -7150,7 +7042,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Y2_33</t>
+          <t>2021_33</t>
         </is>
       </c>
       <c r="C226" t="n">
@@ -7180,7 +7072,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Y2_34</t>
+          <t>2021_34</t>
         </is>
       </c>
       <c r="C227" t="n">
@@ -7200,10 +7092,8 @@
       <c r="G227" t="n">
         <v>0.2410736112946726</v>
       </c>
-      <c r="H227" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H227" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="228">
@@ -7212,7 +7102,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Y2_35</t>
+          <t>2021_35</t>
         </is>
       </c>
       <c r="C228" t="n">
@@ -7232,10 +7122,8 @@
       <c r="G228" t="n">
         <v>0.05591322908249119</v>
       </c>
-      <c r="H228" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H228" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="229">
@@ -7244,7 +7132,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Y2_36</t>
+          <t>2021_36</t>
         </is>
       </c>
       <c r="C229" t="n">
@@ -7264,10 +7152,8 @@
       <c r="G229" t="n">
         <v>0.004782685623373539</v>
       </c>
-      <c r="H229" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H229" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="230">
@@ -7276,7 +7162,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Y2_37</t>
+          <t>2021_37</t>
         </is>
       </c>
       <c r="C230" t="n">
@@ -7304,7 +7190,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Y2_38</t>
+          <t>2021_38</t>
         </is>
       </c>
       <c r="C231" t="n">
@@ -7332,7 +7218,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Y2_39</t>
+          <t>2021_39</t>
         </is>
       </c>
       <c r="C232" t="n">
@@ -7360,7 +7246,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Y2_40</t>
+          <t>2021_40</t>
         </is>
       </c>
       <c r="C233" t="n">
@@ -7388,7 +7274,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Y2_41</t>
+          <t>2021_41</t>
         </is>
       </c>
       <c r="C234" t="n">
@@ -7416,7 +7302,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Y2_42</t>
+          <t>2021_42</t>
         </is>
       </c>
       <c r="C235" t="n">
@@ -7444,7 +7330,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Y2_43</t>
+          <t>2021_43</t>
         </is>
       </c>
       <c r="C236" t="n">
@@ -7472,7 +7358,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Y2_44</t>
+          <t>2021_44</t>
         </is>
       </c>
       <c r="C237" t="n">
@@ -7500,7 +7386,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Y2_45</t>
+          <t>2021_45</t>
         </is>
       </c>
       <c r="C238" t="n">
@@ -7528,7 +7414,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Y2_46</t>
+          <t>2021_46</t>
         </is>
       </c>
       <c r="C239" t="n">
@@ -7556,7 +7442,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Y2_47</t>
+          <t>2021_47</t>
         </is>
       </c>
       <c r="C240" t="n">
@@ -7584,7 +7470,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Y2_48</t>
+          <t>2021_48</t>
         </is>
       </c>
       <c r="C241" t="n">
@@ -7612,7 +7498,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Y3_1</t>
+          <t>2022_1</t>
         </is>
       </c>
       <c r="C242" t="n">
@@ -7640,7 +7526,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Y3_2</t>
+          <t>2022_2</t>
         </is>
       </c>
       <c r="C243" t="n">
@@ -7670,7 +7556,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Y3_3</t>
+          <t>2022_3</t>
         </is>
       </c>
       <c r="C244" t="n">
@@ -7700,7 +7586,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Y3_4</t>
+          <t>2022_4</t>
         </is>
       </c>
       <c r="C245" t="n">
@@ -7730,7 +7616,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Y3_5</t>
+          <t>2022_5</t>
         </is>
       </c>
       <c r="C246" t="n">
@@ -7760,7 +7646,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Y3_6</t>
+          <t>2022_6</t>
         </is>
       </c>
       <c r="C247" t="n">
@@ -7780,10 +7666,8 @@
       <c r="G247" t="n">
         <v>0.2416453465075547</v>
       </c>
-      <c r="H247" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H247" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="248">
@@ -7792,7 +7676,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Y3_7</t>
+          <t>2022_7</t>
         </is>
       </c>
       <c r="C248" t="n">
@@ -7812,10 +7696,8 @@
       <c r="G248" t="n">
         <v>0.05207364194015016</v>
       </c>
-      <c r="H248" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H248" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="249">
@@ -7824,7 +7706,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Y3_8</t>
+          <t>2022_8</t>
         </is>
       </c>
       <c r="C249" t="n">
@@ -7844,10 +7726,8 @@
       <c r="G249" t="n">
         <v>0.004269108485438675</v>
       </c>
-      <c r="H249" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H249" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="250">
@@ -7856,7 +7736,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Y3_9</t>
+          <t>2022_9</t>
         </is>
       </c>
       <c r="C250" t="n">
@@ -7884,7 +7764,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Y3_10</t>
+          <t>2022_10</t>
         </is>
       </c>
       <c r="C251" t="n">
@@ -7912,7 +7792,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Y3_11</t>
+          <t>2022_11</t>
         </is>
       </c>
       <c r="C252" t="n">
@@ -7940,7 +7820,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Y3_12</t>
+          <t>2022_12</t>
         </is>
       </c>
       <c r="C253" t="n">
@@ -7968,7 +7848,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Y3_13</t>
+          <t>2022_13</t>
         </is>
       </c>
       <c r="C254" t="n">
@@ -7996,7 +7876,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Y3_14</t>
+          <t>2022_14</t>
         </is>
       </c>
       <c r="C255" t="n">
@@ -8024,7 +7904,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Y3_15</t>
+          <t>2022_15</t>
         </is>
       </c>
       <c r="C256" t="n">
@@ -8052,7 +7932,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Y3_16</t>
+          <t>2022_16</t>
         </is>
       </c>
       <c r="C257" t="n">
@@ -8080,7 +7960,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Y3_17</t>
+          <t>2022_17</t>
         </is>
       </c>
       <c r="C258" t="n">
@@ -8108,7 +7988,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Y3_18</t>
+          <t>2022_18</t>
         </is>
       </c>
       <c r="C259" t="n">
@@ -8136,7 +8016,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Y3_19</t>
+          <t>2022_19</t>
         </is>
       </c>
       <c r="C260" t="n">
@@ -8164,7 +8044,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Y3_20</t>
+          <t>2022_20</t>
         </is>
       </c>
       <c r="C261" t="n">
@@ -8192,7 +8072,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Y3_21</t>
+          <t>2022_21</t>
         </is>
       </c>
       <c r="C262" t="n">
@@ -8220,7 +8100,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Y3_22</t>
+          <t>2022_22</t>
         </is>
       </c>
       <c r="C263" t="n">
@@ -8250,7 +8130,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Y3_23</t>
+          <t>2022_23</t>
         </is>
       </c>
       <c r="C264" t="n">
@@ -8280,7 +8160,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Y3_24</t>
+          <t>2022_24</t>
         </is>
       </c>
       <c r="C265" t="n">
@@ -8310,7 +8190,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Y3_25</t>
+          <t>2022_25</t>
         </is>
       </c>
       <c r="C266" t="n">
@@ -8340,7 +8220,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Y3_26</t>
+          <t>2022_26</t>
         </is>
       </c>
       <c r="C267" t="n">
@@ -8360,10 +8240,8 @@
       <c r="G267" t="n">
         <v>0.2447799878721271</v>
       </c>
-      <c r="H267" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H267" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="268">
@@ -8372,7 +8250,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Y3_27</t>
+          <t>2022_27</t>
         </is>
       </c>
       <c r="C268" t="n">
@@ -8392,10 +8270,8 @@
       <c r="G268" t="n">
         <v>0.05588401618049743</v>
       </c>
-      <c r="H268" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H268" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="269">
@@ -8404,7 +8280,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Y3_28</t>
+          <t>2022_28</t>
         </is>
       </c>
       <c r="C269" t="n">
@@ -8424,10 +8300,8 @@
       <c r="G269" t="n">
         <v>0.004779951649995142</v>
       </c>
-      <c r="H269" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H269" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="270">
@@ -8436,7 +8310,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Y3_29</t>
+          <t>2022_29</t>
         </is>
       </c>
       <c r="C270" t="n">
@@ -8464,7 +8338,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Y3_30</t>
+          <t>2022_30</t>
         </is>
       </c>
       <c r="C271" t="n">
@@ -8492,7 +8366,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Y3_31</t>
+          <t>2022_31</t>
         </is>
       </c>
       <c r="C272" t="n">
@@ -8520,7 +8394,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Y3_32</t>
+          <t>2022_32</t>
         </is>
       </c>
       <c r="C273" t="n">
@@ -8548,7 +8422,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Y3_33</t>
+          <t>2022_33</t>
         </is>
       </c>
       <c r="C274" t="n">
@@ -8576,7 +8450,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Y3_34</t>
+          <t>2022_34</t>
         </is>
       </c>
       <c r="C275" t="n">
@@ -8604,7 +8478,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Y3_35</t>
+          <t>2022_35</t>
         </is>
       </c>
       <c r="C276" t="n">
@@ -8632,7 +8506,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Y3_36</t>
+          <t>2022_36</t>
         </is>
       </c>
       <c r="C277" t="n">
@@ -8660,7 +8534,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Y3_37</t>
+          <t>2022_37</t>
         </is>
       </c>
       <c r="C278" t="n">
@@ -8688,7 +8562,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Y3_38</t>
+          <t>2022_38</t>
         </is>
       </c>
       <c r="C279" t="n">
@@ -8716,7 +8590,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Y3_39</t>
+          <t>2022_39</t>
         </is>
       </c>
       <c r="C280" t="n">
@@ -8744,7 +8618,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Y3_40</t>
+          <t>2022_40</t>
         </is>
       </c>
       <c r="C281" t="n">
@@ -8772,7 +8646,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Y3_41</t>
+          <t>2022_41</t>
         </is>
       </c>
       <c r="C282" t="n">
@@ -8800,7 +8674,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Y3_42</t>
+          <t>2022_42</t>
         </is>
       </c>
       <c r="C283" t="n">
@@ -8830,7 +8704,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Y3_43</t>
+          <t>2022_43</t>
         </is>
       </c>
       <c r="C284" t="n">
@@ -8860,7 +8734,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Y3_44</t>
+          <t>2022_44</t>
         </is>
       </c>
       <c r="C285" t="n">
@@ -8890,7 +8764,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Y3_45</t>
+          <t>2022_45</t>
         </is>
       </c>
       <c r="C286" t="n">
@@ -8920,7 +8794,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Y3_46</t>
+          <t>2022_46</t>
         </is>
       </c>
       <c r="C287" t="n">
@@ -8940,10 +8814,8 @@
       <c r="G287" t="n">
         <v>0.2599367217400463</v>
       </c>
-      <c r="H287" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H287" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="288">
@@ -8952,7 +8824,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Y3_47</t>
+          <t>2022_47</t>
         </is>
       </c>
       <c r="C288" t="n">
@@ -8972,10 +8844,8 @@
       <c r="G288" t="n">
         <v>0.05837678463661158</v>
       </c>
-      <c r="H288" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H288" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="289">
@@ -8984,7 +8854,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Y3_48</t>
+          <t>2022_48</t>
         </is>
       </c>
       <c r="C289" t="n">
@@ -9004,10 +8874,8 @@
       <c r="G289" t="n">
         <v>0.004885046806971959</v>
       </c>
-      <c r="H289" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="H289" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="290">
@@ -9016,7 +8884,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Y1_1</t>
+          <t>2020_1</t>
         </is>
       </c>
       <c r="C290" t="n">
@@ -9046,7 +8914,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Y1_2</t>
+          <t>2020_2</t>
         </is>
       </c>
       <c r="C291" t="n">
@@ -9076,7 +8944,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Y1_3</t>
+          <t>2020_3</t>
         </is>
       </c>
       <c r="C292" t="n">
@@ -9106,7 +8974,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Y1_4</t>
+          <t>2020_4</t>
         </is>
       </c>
       <c r="C293" t="n">
@@ -9136,7 +9004,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Y1_5</t>
+          <t>2020_5</t>
         </is>
       </c>
       <c r="C294" t="n">
@@ -9166,7 +9034,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Y1_6</t>
+          <t>2020_6</t>
         </is>
       </c>
       <c r="C295" t="n">
@@ -9196,7 +9064,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Y1_7</t>
+          <t>2020_7</t>
         </is>
       </c>
       <c r="C296" t="n">
@@ -9226,7 +9094,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Y1_8</t>
+          <t>2020_8</t>
         </is>
       </c>
       <c r="C297" t="n">
@@ -9256,7 +9124,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Y1_9</t>
+          <t>2020_9</t>
         </is>
       </c>
       <c r="C298" t="n">
@@ -9286,7 +9154,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Y1_10</t>
+          <t>2020_10</t>
         </is>
       </c>
       <c r="C299" t="n">
@@ -9316,7 +9184,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Y1_11</t>
+          <t>2020_11</t>
         </is>
       </c>
       <c r="C300" t="n">
@@ -9346,7 +9214,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Y1_12</t>
+          <t>2020_12</t>
         </is>
       </c>
       <c r="C301" t="n">
@@ -9376,7 +9244,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Y1_13</t>
+          <t>2020_13</t>
         </is>
       </c>
       <c r="C302" t="n">
@@ -9406,7 +9274,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Y1_14</t>
+          <t>2020_14</t>
         </is>
       </c>
       <c r="C303" t="n">
@@ -9436,7 +9304,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Y1_15</t>
+          <t>2020_15</t>
         </is>
       </c>
       <c r="C304" t="n">
@@ -9466,7 +9334,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Y1_16</t>
+          <t>2020_16</t>
         </is>
       </c>
       <c r="C305" t="n">
@@ -9496,7 +9364,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Y1_17</t>
+          <t>2020_17</t>
         </is>
       </c>
       <c r="C306" t="n">
@@ -9526,7 +9394,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Y1_18</t>
+          <t>2020_18</t>
         </is>
       </c>
       <c r="C307" t="n">
@@ -9556,7 +9424,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Y1_19</t>
+          <t>2020_19</t>
         </is>
       </c>
       <c r="C308" t="n">
@@ -9586,7 +9454,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Y1_20</t>
+          <t>2020_20</t>
         </is>
       </c>
       <c r="C309" t="n">
@@ -9616,7 +9484,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Y1_21</t>
+          <t>2020_21</t>
         </is>
       </c>
       <c r="C310" t="n">
@@ -9646,7 +9514,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Y1_22</t>
+          <t>2020_22</t>
         </is>
       </c>
       <c r="C311" t="n">
@@ -9676,7 +9544,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Y1_23</t>
+          <t>2020_23</t>
         </is>
       </c>
       <c r="C312" t="n">
@@ -9706,7 +9574,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Y1_24</t>
+          <t>2020_24</t>
         </is>
       </c>
       <c r="C313" t="n">
@@ -9736,7 +9604,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Y1_25</t>
+          <t>2020_25</t>
         </is>
       </c>
       <c r="C314" t="n">
@@ -9766,7 +9634,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Y1_26</t>
+          <t>2020_26</t>
         </is>
       </c>
       <c r="C315" t="n">
@@ -9796,7 +9664,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Y1_27</t>
+          <t>2020_27</t>
         </is>
       </c>
       <c r="C316" t="n">
@@ -9826,7 +9694,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Y1_28</t>
+          <t>2020_28</t>
         </is>
       </c>
       <c r="C317" t="n">
@@ -9856,7 +9724,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Y1_29</t>
+          <t>2020_29</t>
         </is>
       </c>
       <c r="C318" t="n">
@@ -9886,7 +9754,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Y1_30</t>
+          <t>2020_30</t>
         </is>
       </c>
       <c r="C319" t="n">
@@ -9916,7 +9784,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Y1_31</t>
+          <t>2020_31</t>
         </is>
       </c>
       <c r="C320" t="n">
@@ -9946,7 +9814,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Y1_32</t>
+          <t>2020_32</t>
         </is>
       </c>
       <c r="C321" t="n">
@@ -9976,7 +9844,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Y1_33</t>
+          <t>2020_33</t>
         </is>
       </c>
       <c r="C322" t="n">
@@ -10006,7 +9874,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Y1_34</t>
+          <t>2020_34</t>
         </is>
       </c>
       <c r="C323" t="n">
@@ -10036,7 +9904,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Y1_35</t>
+          <t>2020_35</t>
         </is>
       </c>
       <c r="C324" t="n">
@@ -10066,7 +9934,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Y1_36</t>
+          <t>2020_36</t>
         </is>
       </c>
       <c r="C325" t="n">
@@ -10096,7 +9964,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Y1_37</t>
+          <t>2020_37</t>
         </is>
       </c>
       <c r="C326" t="n">
@@ -10126,7 +9994,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Y1_38</t>
+          <t>2020_38</t>
         </is>
       </c>
       <c r="C327" t="n">
@@ -10156,7 +10024,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Y1_39</t>
+          <t>2020_39</t>
         </is>
       </c>
       <c r="C328" t="n">
@@ -10186,7 +10054,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Y1_40</t>
+          <t>2020_40</t>
         </is>
       </c>
       <c r="C329" t="n">
@@ -10216,7 +10084,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Y1_41</t>
+          <t>2020_41</t>
         </is>
       </c>
       <c r="C330" t="n">
@@ -10246,7 +10114,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Y1_42</t>
+          <t>2020_42</t>
         </is>
       </c>
       <c r="C331" t="n">
@@ -10276,7 +10144,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Y1_43</t>
+          <t>2020_43</t>
         </is>
       </c>
       <c r="C332" t="n">
@@ -10306,7 +10174,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Y1_44</t>
+          <t>2020_44</t>
         </is>
       </c>
       <c r="C333" t="n">
@@ -10336,7 +10204,7 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>Y1_45</t>
+          <t>2020_45</t>
         </is>
       </c>
       <c r="C334" t="n">
@@ -10366,7 +10234,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>Y1_46</t>
+          <t>2020_46</t>
         </is>
       </c>
       <c r="C335" t="n">
@@ -10396,7 +10264,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>Y1_47</t>
+          <t>2020_47</t>
         </is>
       </c>
       <c r="C336" t="n">
@@ -10426,7 +10294,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>Y1_48</t>
+          <t>2020_48</t>
         </is>
       </c>
       <c r="C337" t="n">
@@ -10456,7 +10324,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>Y2_1</t>
+          <t>2021_1</t>
         </is>
       </c>
       <c r="C338" t="n">
@@ -10486,7 +10354,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>Y2_2</t>
+          <t>2021_2</t>
         </is>
       </c>
       <c r="C339" t="n">
@@ -10516,7 +10384,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>Y2_3</t>
+          <t>2021_3</t>
         </is>
       </c>
       <c r="C340" t="n">
@@ -10546,7 +10414,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>Y2_4</t>
+          <t>2021_4</t>
         </is>
       </c>
       <c r="C341" t="n">
@@ -10576,7 +10444,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>Y2_5</t>
+          <t>2021_5</t>
         </is>
       </c>
       <c r="C342" t="n">
@@ -10606,7 +10474,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>Y2_6</t>
+          <t>2021_6</t>
         </is>
       </c>
       <c r="C343" t="n">
@@ -10636,7 +10504,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>Y2_7</t>
+          <t>2021_7</t>
         </is>
       </c>
       <c r="C344" t="n">
@@ -10666,7 +10534,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>Y2_8</t>
+          <t>2021_8</t>
         </is>
       </c>
       <c r="C345" t="n">
@@ -10696,7 +10564,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>Y2_9</t>
+          <t>2021_9</t>
         </is>
       </c>
       <c r="C346" t="n">
@@ -10726,7 +10594,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>Y2_10</t>
+          <t>2021_10</t>
         </is>
       </c>
       <c r="C347" t="n">
@@ -10756,7 +10624,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>Y2_11</t>
+          <t>2021_11</t>
         </is>
       </c>
       <c r="C348" t="n">
@@ -10786,7 +10654,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>Y2_12</t>
+          <t>2021_12</t>
         </is>
       </c>
       <c r="C349" t="n">
@@ -10816,7 +10684,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>Y2_13</t>
+          <t>2021_13</t>
         </is>
       </c>
       <c r="C350" t="n">
@@ -10846,7 +10714,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>Y2_14</t>
+          <t>2021_14</t>
         </is>
       </c>
       <c r="C351" t="n">
@@ -10876,7 +10744,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>Y2_15</t>
+          <t>2021_15</t>
         </is>
       </c>
       <c r="C352" t="n">
@@ -10906,7 +10774,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Y2_16</t>
+          <t>2021_16</t>
         </is>
       </c>
       <c r="C353" t="n">
@@ -10936,7 +10804,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Y2_17</t>
+          <t>2021_17</t>
         </is>
       </c>
       <c r="C354" t="n">
@@ -10966,7 +10834,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Y2_18</t>
+          <t>2021_18</t>
         </is>
       </c>
       <c r="C355" t="n">
@@ -10996,7 +10864,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>Y2_19</t>
+          <t>2021_19</t>
         </is>
       </c>
       <c r="C356" t="n">
@@ -11026,7 +10894,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>Y2_20</t>
+          <t>2021_20</t>
         </is>
       </c>
       <c r="C357" t="n">
@@ -11056,7 +10924,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>Y2_21</t>
+          <t>2021_21</t>
         </is>
       </c>
       <c r="C358" t="n">
@@ -11086,7 +10954,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>Y2_22</t>
+          <t>2021_22</t>
         </is>
       </c>
       <c r="C359" t="n">
@@ -11116,7 +10984,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>Y2_23</t>
+          <t>2021_23</t>
         </is>
       </c>
       <c r="C360" t="n">
@@ -11146,7 +11014,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>Y2_24</t>
+          <t>2021_24</t>
         </is>
       </c>
       <c r="C361" t="n">
@@ -11176,7 +11044,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>Y2_25</t>
+          <t>2021_25</t>
         </is>
       </c>
       <c r="C362" t="n">
@@ -11206,7 +11074,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>Y2_26</t>
+          <t>2021_26</t>
         </is>
       </c>
       <c r="C363" t="n">
@@ -11236,7 +11104,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>Y2_27</t>
+          <t>2021_27</t>
         </is>
       </c>
       <c r="C364" t="n">
@@ -11266,7 +11134,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>Y2_28</t>
+          <t>2021_28</t>
         </is>
       </c>
       <c r="C365" t="n">
@@ -11296,7 +11164,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>Y2_29</t>
+          <t>2021_29</t>
         </is>
       </c>
       <c r="C366" t="n">
@@ -11326,7 +11194,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>Y2_30</t>
+          <t>2021_30</t>
         </is>
       </c>
       <c r="C367" t="n">
@@ -11356,7 +11224,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>Y2_31</t>
+          <t>2021_31</t>
         </is>
       </c>
       <c r="C368" t="n">
@@ -11386,7 +11254,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>Y2_32</t>
+          <t>2021_32</t>
         </is>
       </c>
       <c r="C369" t="n">
@@ -11416,7 +11284,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>Y2_33</t>
+          <t>2021_33</t>
         </is>
       </c>
       <c r="C370" t="n">
@@ -11446,7 +11314,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>Y2_34</t>
+          <t>2021_34</t>
         </is>
       </c>
       <c r="C371" t="n">
@@ -11476,7 +11344,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>Y2_35</t>
+          <t>2021_35</t>
         </is>
       </c>
       <c r="C372" t="n">
@@ -11506,7 +11374,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>Y2_36</t>
+          <t>2021_36</t>
         </is>
       </c>
       <c r="C373" t="n">
@@ -11536,7 +11404,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>Y2_37</t>
+          <t>2021_37</t>
         </is>
       </c>
       <c r="C374" t="n">
@@ -11566,7 +11434,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>Y2_38</t>
+          <t>2021_38</t>
         </is>
       </c>
       <c r="C375" t="n">
@@ -11596,7 +11464,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>Y2_39</t>
+          <t>2021_39</t>
         </is>
       </c>
       <c r="C376" t="n">
@@ -11626,7 +11494,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>Y2_40</t>
+          <t>2021_40</t>
         </is>
       </c>
       <c r="C377" t="n">
@@ -11656,7 +11524,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>Y2_41</t>
+          <t>2021_41</t>
         </is>
       </c>
       <c r="C378" t="n">
@@ -11686,7 +11554,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>Y2_42</t>
+          <t>2021_42</t>
         </is>
       </c>
       <c r="C379" t="n">
@@ -11716,7 +11584,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Y2_43</t>
+          <t>2021_43</t>
         </is>
       </c>
       <c r="C380" t="n">
@@ -11746,7 +11614,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Y2_44</t>
+          <t>2021_44</t>
         </is>
       </c>
       <c r="C381" t="n">
@@ -11776,7 +11644,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>Y2_45</t>
+          <t>2021_45</t>
         </is>
       </c>
       <c r="C382" t="n">
@@ -11806,7 +11674,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>Y2_46</t>
+          <t>2021_46</t>
         </is>
       </c>
       <c r="C383" t="n">
@@ -11836,7 +11704,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>Y2_47</t>
+          <t>2021_47</t>
         </is>
       </c>
       <c r="C384" t="n">
@@ -11866,7 +11734,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>Y2_48</t>
+          <t>2021_48</t>
         </is>
       </c>
       <c r="C385" t="n">
@@ -11896,7 +11764,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>Y3_1</t>
+          <t>2022_1</t>
         </is>
       </c>
       <c r="C386" t="n">
@@ -11926,7 +11794,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>Y3_2</t>
+          <t>2022_2</t>
         </is>
       </c>
       <c r="C387" t="n">
@@ -11956,7 +11824,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>Y3_3</t>
+          <t>2022_3</t>
         </is>
       </c>
       <c r="C388" t="n">
@@ -11986,7 +11854,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>Y3_4</t>
+          <t>2022_4</t>
         </is>
       </c>
       <c r="C389" t="n">
@@ -12016,7 +11884,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>Y3_5</t>
+          <t>2022_5</t>
         </is>
       </c>
       <c r="C390" t="n">
@@ -12046,7 +11914,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>Y3_6</t>
+          <t>2022_6</t>
         </is>
       </c>
       <c r="C391" t="n">
@@ -12076,7 +11944,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>Y3_7</t>
+          <t>2022_7</t>
         </is>
       </c>
       <c r="C392" t="n">
@@ -12106,7 +11974,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>Y3_8</t>
+          <t>2022_8</t>
         </is>
       </c>
       <c r="C393" t="n">
@@ -12136,7 +12004,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Y3_9</t>
+          <t>2022_9</t>
         </is>
       </c>
       <c r="C394" t="n">
@@ -12166,7 +12034,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>Y3_10</t>
+          <t>2022_10</t>
         </is>
       </c>
       <c r="C395" t="n">
@@ -12196,7 +12064,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>Y3_11</t>
+          <t>2022_11</t>
         </is>
       </c>
       <c r="C396" t="n">
@@ -12226,7 +12094,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>Y3_12</t>
+          <t>2022_12</t>
         </is>
       </c>
       <c r="C397" t="n">
@@ -12256,7 +12124,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>Y3_13</t>
+          <t>2022_13</t>
         </is>
       </c>
       <c r="C398" t="n">
@@ -12286,7 +12154,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>Y3_14</t>
+          <t>2022_14</t>
         </is>
       </c>
       <c r="C399" t="n">
@@ -12316,7 +12184,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>Y3_15</t>
+          <t>2022_15</t>
         </is>
       </c>
       <c r="C400" t="n">
@@ -12346,7 +12214,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>Y3_16</t>
+          <t>2022_16</t>
         </is>
       </c>
       <c r="C401" t="n">
@@ -12376,7 +12244,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>Y3_17</t>
+          <t>2022_17</t>
         </is>
       </c>
       <c r="C402" t="n">
@@ -12406,7 +12274,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>Y3_18</t>
+          <t>2022_18</t>
         </is>
       </c>
       <c r="C403" t="n">
@@ -12436,7 +12304,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>Y3_19</t>
+          <t>2022_19</t>
         </is>
       </c>
       <c r="C404" t="n">
@@ -12466,7 +12334,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>Y3_20</t>
+          <t>2022_20</t>
         </is>
       </c>
       <c r="C405" t="n">
@@ -12496,7 +12364,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>Y3_21</t>
+          <t>2022_21</t>
         </is>
       </c>
       <c r="C406" t="n">
@@ -12526,7 +12394,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>Y3_22</t>
+          <t>2022_22</t>
         </is>
       </c>
       <c r="C407" t="n">
@@ -12556,7 +12424,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Y3_23</t>
+          <t>2022_23</t>
         </is>
       </c>
       <c r="C408" t="n">
@@ -12586,7 +12454,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>Y3_24</t>
+          <t>2022_24</t>
         </is>
       </c>
       <c r="C409" t="n">
@@ -12616,7 +12484,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Y3_25</t>
+          <t>2022_25</t>
         </is>
       </c>
       <c r="C410" t="n">
@@ -12646,7 +12514,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Y3_26</t>
+          <t>2022_26</t>
         </is>
       </c>
       <c r="C411" t="n">
@@ -12676,7 +12544,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Y3_27</t>
+          <t>2022_27</t>
         </is>
       </c>
       <c r="C412" t="n">
@@ -12706,7 +12574,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>Y3_28</t>
+          <t>2022_28</t>
         </is>
       </c>
       <c r="C413" t="n">
@@ -12736,7 +12604,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>Y3_29</t>
+          <t>2022_29</t>
         </is>
       </c>
       <c r="C414" t="n">
@@ -12766,7 +12634,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>Y3_30</t>
+          <t>2022_30</t>
         </is>
       </c>
       <c r="C415" t="n">
@@ -12796,7 +12664,7 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>Y3_31</t>
+          <t>2022_31</t>
         </is>
       </c>
       <c r="C416" t="n">
@@ -12826,7 +12694,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>Y3_32</t>
+          <t>2022_32</t>
         </is>
       </c>
       <c r="C417" t="n">
@@ -12856,7 +12724,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>Y3_33</t>
+          <t>2022_33</t>
         </is>
       </c>
       <c r="C418" t="n">
@@ -12886,7 +12754,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>Y3_34</t>
+          <t>2022_34</t>
         </is>
       </c>
       <c r="C419" t="n">
@@ -12916,7 +12784,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>Y3_35</t>
+          <t>2022_35</t>
         </is>
       </c>
       <c r="C420" t="n">
@@ -12946,7 +12814,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>Y3_36</t>
+          <t>2022_36</t>
         </is>
       </c>
       <c r="C421" t="n">
@@ -12976,7 +12844,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>Y3_37</t>
+          <t>2022_37</t>
         </is>
       </c>
       <c r="C422" t="n">
@@ -13006,7 +12874,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>Y3_38</t>
+          <t>2022_38</t>
         </is>
       </c>
       <c r="C423" t="n">
@@ -13036,7 +12904,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>Y3_39</t>
+          <t>2022_39</t>
         </is>
       </c>
       <c r="C424" t="n">
@@ -13066,7 +12934,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>Y3_40</t>
+          <t>2022_40</t>
         </is>
       </c>
       <c r="C425" t="n">
@@ -13096,7 +12964,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>Y3_41</t>
+          <t>2022_41</t>
         </is>
       </c>
       <c r="C426" t="n">
@@ -13126,7 +12994,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>Y3_42</t>
+          <t>2022_42</t>
         </is>
       </c>
       <c r="C427" t="n">
@@ -13156,7 +13024,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>Y3_43</t>
+          <t>2022_43</t>
         </is>
       </c>
       <c r="C428" t="n">
@@ -13186,7 +13054,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>Y3_44</t>
+          <t>2022_44</t>
         </is>
       </c>
       <c r="C429" t="n">
@@ -13216,7 +13084,7 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>Y3_45</t>
+          <t>2022_45</t>
         </is>
       </c>
       <c r="C430" t="n">
@@ -13246,7 +13114,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>Y3_46</t>
+          <t>2022_46</t>
         </is>
       </c>
       <c r="C431" t="n">
@@ -13276,7 +13144,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>Y3_47</t>
+          <t>2022_47</t>
         </is>
       </c>
       <c r="C432" t="n">
@@ -13306,7 +13174,7 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>Y3_48</t>
+          <t>2022_48</t>
         </is>
       </c>
       <c r="C433" t="n">

</xml_diff>